<commit_message>
Early work on hypergolic fuel implementation
</commit_message>
<xml_diff>
--- a/Plotting/0.7.5/DSSHU.xlsx
+++ b/Plotting/0.7.5/DSSHU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkScienceSystem\Plotting\0.7.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkScienceSystem\Plotting\0.7.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D04321-69AC-43EB-A51B-553CF8583296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94171CCC-40A8-457B-A34F-025F1BFEAFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="15192" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7584" yWindow="1164" windowWidth="15228" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSSHU" sheetId="1" r:id="rId1"/>
@@ -904,10 +904,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -929,6 +932,9 @@
       </c>
       <c r="B2" t="s">
         <v>9</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -940,7 +946,7 @@
 }"</f>
         <v>@PART[HDUConnector]:AFTER[DSSHU] //
 {
-	@TechRequired = bases
+	@TechRequired = bases10
 }</v>
       </c>
     </row>
@@ -950,6 +956,9 @@
       </c>
       <c r="B3" t="s">
         <v>9</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -961,7 +970,7 @@
 }"</f>
         <v>@PART[HDU1]:AFTER[DSSHU] //
 {
-	@TechRequired = bases
+	@TechRequired = bases10
 }</v>
       </c>
     </row>
@@ -972,6 +981,9 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
@@ -979,7 +991,7 @@
         <f t="shared" si="1"/>
         <v>@PART[HDU2]:AFTER[DSSHU] //
 {
-	@TechRequired = bases
+	@TechRequired = bases10
 }</v>
       </c>
     </row>
@@ -990,6 +1002,9 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
@@ -997,7 +1012,7 @@
         <f t="shared" si="1"/>
         <v>@PART[HDU3]:AFTER[DSSHU] //
 {
-	@TechRequired = bases
+	@TechRequired = bases10
 }</v>
       </c>
     </row>

</xml_diff>